<commit_message>
Wyniki - zakazenia w trkaice
</commit_message>
<xml_diff>
--- a/Skutecznosc kultur ratunkowych.xlsx
+++ b/Skutecznosc kultur ratunkowych.xlsx
@@ -1,18 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48A86E-F8E6-4776-9395-544B98AA01CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3213EA71-D0D8-46B7-B55B-286D19A1D013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skutecnzosc kultur taunkowych" sheetId="6" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1459,91 +1456,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Zakazenia zbiorczy"/>
-      <sheetName val="Zakazenia baza"/>
-      <sheetName val="Sniezyca podsumowanie"/>
-      <sheetName val="Szachownica podsumowanie"/>
-      <sheetName val="Pozywka z antybiotykiem"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>Pozywka bez antybiotyku</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>Pozywka z antybiotykiem</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Działki okwiatu</v>
-          </cell>
-          <cell r="F6">
-            <v>30</v>
-          </cell>
-          <cell r="J6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Liść</v>
-          </cell>
-          <cell r="F7">
-            <v>10</v>
-          </cell>
-          <cell r="J7">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Łodyga nadziemna</v>
-          </cell>
-          <cell r="F8">
-            <v>26</v>
-          </cell>
-          <cell r="J8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Łuska</v>
-          </cell>
-          <cell r="F9">
-            <v>42.5</v>
-          </cell>
-          <cell r="J9">
-            <v>27.058823529411764</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Piętka</v>
-          </cell>
-          <cell r="F10">
-            <v>48.571428571428569</v>
-          </cell>
-          <cell r="J10">
-            <v>100</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1810,7 +1722,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>